<commit_message>
Update today's matches data
</commit_message>
<xml_diff>
--- a/data/todays_matches/todays_matches.xlsx
+++ b/data/todays_matches/todays_matches.xlsx
@@ -134,6 +134,47 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MatchesTable" displayName="MatchesTable" ref="A1:AF35" headerRowCount="1">
+  <autoFilter ref="A1:AF35"/>
+  <tableColumns count="32">
+    <tableColumn id="1" name="date"/>
+    <tableColumn id="2" name="game_week"/>
+    <tableColumn id="3" name="home_name"/>
+    <tableColumn id="4" name="away_name"/>
+    <tableColumn id="5" name="pre_match_home_ppg"/>
+    <tableColumn id="6" name="pre_match_away_ppg"/>
+    <tableColumn id="7" name="team_a_xg_prematch"/>
+    <tableColumn id="8" name="team_b_xg_prematch"/>
+    <tableColumn id="9" name="total_xg_prematch"/>
+    <tableColumn id="10" name="btts_potential"/>
+    <tableColumn id="11" name="o05HT_potential"/>
+    <tableColumn id="12" name="o15HT_potential"/>
+    <tableColumn id="13" name="u15_potential"/>
+    <tableColumn id="14" name="o15_potential"/>
+    <tableColumn id="15" name="o25_potential"/>
+    <tableColumn id="16" name="u25_potential"/>
+    <tableColumn id="17" name="odds_ft_1"/>
+    <tableColumn id="18" name="odds_ft_x"/>
+    <tableColumn id="19" name="odds_ft_2"/>
+    <tableColumn id="20" name="odds_ft_over15"/>
+    <tableColumn id="21" name="odds_ft_over25"/>
+    <tableColumn id="22" name="odds_ft_over35"/>
+    <tableColumn id="23" name="odds_btts_yes"/>
+    <tableColumn id="24" name="odds_btts_no"/>
+    <tableColumn id="25" name="odds_corners_under_85"/>
+    <tableColumn id="26" name="odds_corners_under_95"/>
+    <tableColumn id="27" name="odds_corners_over_85"/>
+    <tableColumn id="28" name="odds_corners_over_95"/>
+    <tableColumn id="29" name="odds_1st_half_over05"/>
+    <tableColumn id="30" name="odds_1st_half_over15"/>
+    <tableColumn id="31" name="odds_1st_half_under05"/>
+    <tableColumn id="32" name="odds_1st_half_under15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF22"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,8 +476,8 @@
   <cols>
     <col width="25.2" customWidth="1" min="1" max="1"/>
     <col width="13.2" customWidth="1" min="2" max="2"/>
-    <col width="25.2" customWidth="1" min="3" max="3"/>
-    <col width="26.4" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="21.6" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
     <col width="24" customWidth="1" min="7" max="7"/>
@@ -632,2188 +673,3543 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-05 17:45:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Qarabağ</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Ceará</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2.33</v>
+        <v>1.67</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0.88</v>
       </c>
       <c r="G2" t="n">
-        <v>1.55</v>
+        <v>1.47</v>
       </c>
       <c r="H2" t="n">
-        <v>1.59</v>
+        <v>1.16</v>
       </c>
       <c r="I2" t="n">
-        <v>3.14</v>
+        <v>2.63</v>
       </c>
       <c r="J2" t="n">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K2" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="L2" t="n">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="M2" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="N2" t="n">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="O2" t="n">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="P2" t="n">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="Q2" t="n">
-        <v>8</v>
+        <v>1.62</v>
       </c>
       <c r="R2" t="n">
-        <v>5.25</v>
+        <v>3.09</v>
       </c>
       <c r="S2" t="n">
-        <v>1.36</v>
+        <v>5.6</v>
       </c>
       <c r="T2" t="n">
-        <v>1.11</v>
+        <v>1.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1.47</v>
+        <v>2.45</v>
       </c>
       <c r="V2" t="n">
-        <v>2.28</v>
+        <v>4.25</v>
       </c>
       <c r="W2" t="n">
-        <v>1.77</v>
+        <v>2.14</v>
       </c>
       <c r="X2" t="n">
-        <v>1.95</v>
+        <v>1.63</v>
       </c>
       <c r="Y2" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="AB2" t="n">
         <v>2.03</v>
       </c>
-      <c r="Z2" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="AE2" t="n">
         <v>2.53</v>
       </c>
-      <c r="AC2" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>3.66</v>
-      </c>
       <c r="AF2" t="n">
-        <v>1.65</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-05 17:45:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Paphos</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Fluminense</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.78</v>
+        <v>2.38</v>
       </c>
       <c r="F3" t="n">
-        <v>0.33</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>1.15</v>
+        <v>1.66</v>
       </c>
       <c r="H3" t="n">
-        <v>1.27</v>
+        <v>1.11</v>
       </c>
       <c r="I3" t="n">
-        <v>2.42</v>
+        <v>2.77</v>
       </c>
       <c r="J3" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="K3" t="n">
         <v>72</v>
       </c>
       <c r="L3" t="n">
+        <v>35</v>
+      </c>
+      <c r="M3" t="n">
         <v>22</v>
       </c>
-      <c r="M3" t="n">
-        <v>39</v>
-      </c>
       <c r="N3" t="n">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="O3" t="n">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="P3" t="n">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="Q3" t="n">
-        <v>7.5</v>
+        <v>1.79</v>
       </c>
       <c r="R3" t="n">
-        <v>4.95</v>
+        <v>3.05</v>
       </c>
       <c r="S3" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="T3" t="n">
         <v>1.38</v>
       </c>
-      <c r="T3" t="n">
-        <v>1.2</v>
-      </c>
       <c r="U3" t="n">
-        <v>1.57</v>
+        <v>2.3</v>
       </c>
       <c r="V3" t="n">
-        <v>2.49</v>
+        <v>4.2</v>
       </c>
       <c r="W3" t="n">
-        <v>1.91</v>
+        <v>2.06</v>
       </c>
       <c r="X3" t="n">
-        <v>1.91</v>
+        <v>1.68</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.28</v>
+        <v>2.31</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.8</v>
+        <v>1.87</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.7</v>
+        <v>1.52</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.23</v>
+        <v>1.93</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.28</v>
+        <v>1.44</v>
       </c>
       <c r="AD3" t="n">
-        <v>2.45</v>
+        <v>3.28</v>
       </c>
       <c r="AE3" t="n">
-        <v>3.5</v>
+        <v>2.44</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.5</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-05 19:00:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>33</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Vitória</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Botafogo</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="J4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K4" t="n">
+        <v>60</v>
+      </c>
+      <c r="L4" t="n">
         <v>10</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Real Sociedad II</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>SD Huesca</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2.07</v>
-      </c>
-      <c r="J4" t="n">
-        <v>50</v>
-      </c>
-      <c r="K4" t="n">
-        <v>90</v>
-      </c>
-      <c r="L4" t="n">
-        <v>30</v>
-      </c>
       <c r="M4" t="n">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="N4" t="n">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="O4" t="n">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="P4" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.88</v>
+        <v>2.94</v>
       </c>
       <c r="R4" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="V4" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="AD4" t="n">
         <v>2.9</v>
       </c>
-      <c r="S4" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="U4" t="n">
-        <v>2.56</v>
-      </c>
-      <c r="V4" t="n">
-        <v>5.65</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>1.69</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>2.53</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>3.5</v>
-      </c>
       <c r="AE4" t="n">
-        <v>2.31</v>
+        <v>2.59</v>
       </c>
       <c r="AF4" t="n">
-        <v>1.25</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-05 19:45:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Preston North End</t>
+          <t>Once Caldas</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Swansea City</t>
+          <t>Deportivo Pasto</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="F5" t="n">
-        <v>1.33</v>
+        <v>1.18</v>
       </c>
       <c r="G5" t="n">
-        <v>1.24</v>
+        <v>1.38</v>
       </c>
       <c r="H5" t="n">
-        <v>1.05</v>
+        <v>1.21</v>
       </c>
       <c r="I5" t="n">
-        <v>2.29</v>
+        <v>2.59</v>
       </c>
       <c r="J5" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="K5" t="n">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="L5" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="M5" t="n">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="N5" t="n">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="O5" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="P5" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="Q5" t="n">
-        <v>2.26</v>
+        <v>1.58</v>
       </c>
       <c r="R5" t="n">
-        <v>2.9</v>
+        <v>3.55</v>
       </c>
       <c r="S5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T5" t="n">
-        <v>1.42</v>
+        <v>1.34</v>
       </c>
       <c r="U5" t="n">
-        <v>2.4</v>
+        <v>2.02</v>
       </c>
       <c r="V5" t="n">
-        <v>4.91</v>
+        <v>3.34</v>
       </c>
       <c r="W5" t="n">
-        <v>1.97</v>
+        <v>2.02</v>
       </c>
       <c r="X5" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AB5" t="n">
         <v>1.75</v>
       </c>
-      <c r="Y5" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>2.02</v>
-      </c>
       <c r="AC5" t="n">
-        <v>1.53</v>
+        <v>1.3</v>
       </c>
       <c r="AD5" t="n">
-        <v>3.15</v>
+        <v>2.85</v>
       </c>
       <c r="AE5" t="n">
-        <v>2.34</v>
+        <v>3.05</v>
       </c>
       <c r="AF5" t="n">
-        <v>1.3</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-05 19:45:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sheffield Wednesday</t>
+          <t>Brøndby</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Norwich City</t>
+          <t>Nordsjælland</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.14</v>
+        <v>1.86</v>
       </c>
       <c r="F6" t="n">
-        <v>1.14</v>
+        <v>1.29</v>
       </c>
       <c r="G6" t="n">
-        <v>1.26</v>
+        <v>1.64</v>
       </c>
       <c r="H6" t="n">
-        <v>1.11</v>
+        <v>1.46</v>
       </c>
       <c r="I6" t="n">
-        <v>2.37</v>
+        <v>3.1</v>
       </c>
       <c r="J6" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="K6" t="n">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L6" t="n">
         <v>43</v>
       </c>
       <c r="M6" t="n">
+        <v>7</v>
+      </c>
+      <c r="N6" t="n">
+        <v>93</v>
+      </c>
+      <c r="O6" t="n">
+        <v>86</v>
+      </c>
+      <c r="P6" t="n">
         <v>14</v>
       </c>
-      <c r="N6" t="n">
-        <v>86</v>
-      </c>
-      <c r="O6" t="n">
-        <v>50</v>
-      </c>
-      <c r="P6" t="n">
-        <v>50</v>
-      </c>
       <c r="Q6" t="n">
-        <v>2.98</v>
+        <v>2.15</v>
       </c>
       <c r="R6" t="n">
-        <v>3.45</v>
+        <v>3.4</v>
       </c>
       <c r="S6" t="n">
-        <v>2.22</v>
+        <v>3.28</v>
       </c>
       <c r="T6" t="n">
-        <v>1.26</v>
+        <v>1.22</v>
       </c>
       <c r="U6" t="n">
-        <v>1.85</v>
+        <v>1.58</v>
       </c>
       <c r="V6" t="n">
-        <v>3</v>
+        <v>2.56</v>
       </c>
       <c r="W6" t="n">
-        <v>1.65</v>
+        <v>1.62</v>
       </c>
       <c r="X6" t="n">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.73</v>
+        <v>2.13</v>
       </c>
       <c r="Z6" t="n">
-        <v>2.07</v>
+        <v>1.67</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.37</v>
+        <v>1.66</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.62</v>
+        <v>2.05</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
       <c r="AD6" t="n">
-        <v>2.65</v>
+        <v>2.39</v>
       </c>
       <c r="AE6" t="n">
-        <v>2.99</v>
+        <v>3.55</v>
       </c>
       <c r="AF6" t="n">
-        <v>1.42</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-05 19:45:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Queens Park Rangers</t>
+          <t>Go Ahead Eagles</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>Feyenoord</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1.33</v>
+        <v>1.6</v>
       </c>
       <c r="F7" t="n">
-        <v>0.86</v>
+        <v>2.6</v>
       </c>
       <c r="G7" t="n">
-        <v>1.53</v>
+        <v>1.66</v>
       </c>
       <c r="H7" t="n">
-        <v>1.5</v>
+        <v>2.07</v>
       </c>
       <c r="I7" t="n">
-        <v>3.03</v>
+        <v>3.73</v>
       </c>
       <c r="J7" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="K7" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L7" t="n">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="M7" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N7" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="O7" t="n">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="P7" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.7</v>
+        <v>6.1</v>
       </c>
       <c r="R7" t="n">
-        <v>3.45</v>
+        <v>4.55</v>
       </c>
       <c r="S7" t="n">
-        <v>2.5</v>
+        <v>1.52</v>
       </c>
       <c r="T7" t="n">
-        <v>1.22</v>
+        <v>1.16</v>
       </c>
       <c r="U7" t="n">
-        <v>1.88</v>
+        <v>1.49</v>
       </c>
       <c r="V7" t="n">
-        <v>2.89</v>
+        <v>2.2</v>
       </c>
       <c r="W7" t="n">
-        <v>1.68</v>
+        <v>1.57</v>
       </c>
       <c r="X7" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="Y7" t="n">
-        <v>2.45</v>
+        <v>3.05</v>
       </c>
       <c r="Z7" t="n">
-        <v>1.84</v>
+        <v>2.21</v>
       </c>
       <c r="AA7" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="AB7" t="n">
         <v>1.54</v>
       </c>
-      <c r="AB7" t="n">
-        <v>2.16</v>
-      </c>
       <c r="AC7" t="n">
-        <v>1.38</v>
+        <v>1.25</v>
       </c>
       <c r="AD7" t="n">
-        <v>2.65</v>
+        <v>2.26</v>
       </c>
       <c r="AE7" t="n">
-        <v>3.08</v>
+        <v>4.1</v>
       </c>
       <c r="AF7" t="n">
-        <v>1.43</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:00:00</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Panathinaikos</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Wrexham</t>
+          <t>PAOK</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>1.33</v>
+        <v>2.5</v>
       </c>
       <c r="G8" t="n">
-        <v>1.54</v>
+        <v>1.72</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.58</v>
       </c>
       <c r="I8" t="n">
-        <v>2.48</v>
+        <v>3.3</v>
       </c>
       <c r="J8" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K8" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="L8" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M8" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="N8" t="n">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="O8" t="n">
         <v>38</v>
       </c>
       <c r="P8" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.44</v>
+        <v>2.34</v>
       </c>
       <c r="R8" t="n">
-        <v>3.21</v>
+        <v>3</v>
       </c>
       <c r="S8" t="n">
-        <v>2.57</v>
+        <v>2.89</v>
       </c>
       <c r="T8" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="U8" t="n">
-        <v>2.22</v>
+        <v>2</v>
       </c>
       <c r="V8" t="n">
-        <v>4.01</v>
+        <v>3.6</v>
       </c>
       <c r="W8" t="n">
-        <v>1.83</v>
+        <v>1.75</v>
       </c>
       <c r="X8" t="n">
-        <v>1.93</v>
+        <v>1.95</v>
       </c>
       <c r="Y8" t="n">
-        <v>2.97</v>
+        <v>2.05</v>
       </c>
       <c r="Z8" t="n">
-        <v>2.18</v>
+        <v>1.54</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.32</v>
+        <v>1.81</v>
       </c>
       <c r="AB8" t="n">
-        <v>1.56</v>
+        <v>2.7</v>
       </c>
       <c r="AC8" t="n">
-        <v>1.46</v>
+        <v>1.43</v>
       </c>
       <c r="AD8" t="n">
-        <v>3.23</v>
+        <v>2.88</v>
       </c>
       <c r="AE8" t="n">
-        <v>2.53</v>
+        <v>2.62</v>
       </c>
       <c r="AF8" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:15:00</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Club Brugge</t>
+          <t>Arka Gdynia</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FC Barcelona</t>
+          <t>Lech Poznań</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2.14</v>
+        <v>1.07</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1.62</v>
       </c>
       <c r="G9" t="n">
-        <v>1.88</v>
+        <v>1.14</v>
       </c>
       <c r="H9" t="n">
-        <v>1.68</v>
+        <v>1.83</v>
       </c>
       <c r="I9" t="n">
-        <v>3.56</v>
+        <v>2.97</v>
       </c>
       <c r="J9" t="n">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="K9" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L9" t="n">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="M9" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="N9" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="O9" t="n">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="P9" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="Q9" t="n">
-        <v>5.2</v>
+        <v>4.2</v>
       </c>
       <c r="R9" t="n">
-        <v>5.35</v>
+        <v>3.4</v>
       </c>
       <c r="S9" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="T9" t="n">
-        <v>1.04</v>
+        <v>1.2</v>
       </c>
       <c r="U9" t="n">
-        <v>1.3</v>
+        <v>1.83</v>
       </c>
       <c r="V9" t="n">
-        <v>1.88</v>
+        <v>2.83</v>
       </c>
       <c r="W9" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="X9" t="n">
-        <v>2.95</v>
+        <v>2.13</v>
       </c>
       <c r="Y9" t="n">
-        <v>2.48</v>
+        <v>2.65</v>
       </c>
       <c r="Z9" t="n">
-        <v>1.93</v>
+        <v>2.23</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.51</v>
+        <v>1.37</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.81</v>
+        <v>1.62</v>
       </c>
       <c r="AC9" t="n">
-        <v>1.16</v>
+        <v>1.35</v>
       </c>
       <c r="AD9" t="n">
-        <v>1.88</v>
+        <v>2.5</v>
       </c>
       <c r="AE9" t="n">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="AF9" t="n">
-        <v>1.94</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:30:00</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ajax</t>
+          <t>Boca Juniors</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Galatasaray</t>
+          <t>River Plate</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>1.57</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8</v>
+        <v>1.65</v>
       </c>
       <c r="H10" t="n">
-        <v>1.69</v>
+        <v>1.39</v>
       </c>
       <c r="I10" t="n">
-        <v>2.49</v>
+        <v>3.04</v>
       </c>
       <c r="J10" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="K10" t="n">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="L10" t="n">
+        <v>24</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30</v>
+      </c>
+      <c r="N10" t="n">
+        <v>70</v>
+      </c>
+      <c r="O10" t="n">
+        <v>34</v>
+      </c>
+      <c r="P10" t="n">
         <v>67</v>
       </c>
-      <c r="M10" t="n">
-        <v>17</v>
-      </c>
-      <c r="N10" t="n">
-        <v>84</v>
-      </c>
-      <c r="O10" t="n">
-        <v>67</v>
-      </c>
-      <c r="P10" t="n">
-        <v>33</v>
-      </c>
       <c r="Q10" t="n">
-        <v>3.2</v>
+        <v>2.23</v>
       </c>
       <c r="R10" t="n">
-        <v>3.9</v>
+        <v>2.8</v>
       </c>
       <c r="S10" t="n">
-        <v>2.1</v>
+        <v>3.25</v>
       </c>
       <c r="T10" t="n">
-        <v>1.12</v>
+        <v>1.47</v>
       </c>
       <c r="U10" t="n">
-        <v>1.42</v>
+        <v>2.7</v>
       </c>
       <c r="V10" t="n">
-        <v>2.18</v>
+        <v>4.8</v>
       </c>
       <c r="W10" t="n">
-        <v>1.44</v>
+        <v>2.14</v>
       </c>
       <c r="X10" t="n">
-        <v>2.92</v>
+        <v>1.67</v>
       </c>
       <c r="Y10" t="n">
-        <v>2.21</v>
+        <v>2.05</v>
       </c>
       <c r="Z10" t="n">
-        <v>1.75</v>
+        <v>1.62</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.62</v>
+        <v>1.74</v>
       </c>
       <c r="AB10" t="n">
-        <v>2.31</v>
+        <v>2.61</v>
       </c>
       <c r="AC10" t="n">
-        <v>1.24</v>
+        <v>1.57</v>
       </c>
       <c r="AD10" t="n">
-        <v>2.05</v>
+        <v>3.25</v>
       </c>
       <c r="AE10" t="n">
-        <v>3.84</v>
+        <v>2.22</v>
       </c>
       <c r="AF10" t="n">
-        <v>1.73</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:30:00</t>
         </is>
       </c>
       <c r="B11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Defensor Sporting</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Nacional</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="J11" t="n">
+        <v>50</v>
+      </c>
+      <c r="K11" t="n">
+        <v>59</v>
+      </c>
+      <c r="L11" t="n">
+        <v>37</v>
+      </c>
+      <c r="M11" t="n">
+        <v>33</v>
+      </c>
+      <c r="N11" t="n">
+        <v>67</v>
+      </c>
+      <c r="O11" t="n">
+        <v>54</v>
+      </c>
+      <c r="P11" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q11" t="n">
         <v>4</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Manchester City</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Borussia Dortmund</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.41</v>
-      </c>
-      <c r="I11" t="n">
-        <v>3.61</v>
-      </c>
-      <c r="J11" t="n">
-        <v>67</v>
-      </c>
-      <c r="K11" t="n">
-        <v>67</v>
-      </c>
-      <c r="L11" t="n">
-        <v>50</v>
-      </c>
-      <c r="M11" t="n">
+      <c r="R11" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="T11" t="n">
         <v>0</v>
       </c>
-      <c r="N11" t="n">
-        <v>100</v>
-      </c>
-      <c r="O11" t="n">
-        <v>67</v>
-      </c>
-      <c r="P11" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="R11" t="n">
-        <v>5.45</v>
-      </c>
-      <c r="S11" t="n">
-        <v>6</v>
-      </c>
-      <c r="T11" t="n">
-        <v>1.08</v>
-      </c>
       <c r="U11" t="n">
-        <v>1.41</v>
+        <v>2.05</v>
       </c>
       <c r="V11" t="n">
-        <v>2.14</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>1.53</v>
+        <v>1.83</v>
       </c>
       <c r="X11" t="n">
-        <v>2.3</v>
+        <v>1.83</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.53</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>2.08</v>
+        <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>1.22</v>
+        <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>2.05</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>4.05</v>
+        <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>1.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:30:00</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Benfica</t>
+          <t>Juventud</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Bayer Leverkusen</t>
+          <t>Progreso</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.43</v>
+        <v>1.67</v>
       </c>
       <c r="F12" t="n">
-        <v>0.67</v>
+        <v>1.06</v>
       </c>
       <c r="G12" t="n">
-        <v>1.34</v>
+        <v>1.28</v>
       </c>
       <c r="H12" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="J12" t="n">
+        <v>52</v>
+      </c>
+      <c r="K12" t="n">
+        <v>63</v>
+      </c>
+      <c r="L12" t="n">
+        <v>27</v>
+      </c>
+      <c r="M12" t="n">
+        <v>34</v>
+      </c>
+      <c r="N12" t="n">
+        <v>67</v>
+      </c>
+      <c r="O12" t="n">
+        <v>47</v>
+      </c>
+      <c r="P12" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="R12" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="S12" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="T12" t="n">
         <v>1.26</v>
       </c>
-      <c r="I12" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="J12" t="n">
-        <v>57</v>
-      </c>
-      <c r="K12" t="n">
-        <v>69</v>
-      </c>
-      <c r="L12" t="n">
-        <v>31</v>
-      </c>
-      <c r="M12" t="n">
-        <v>22</v>
-      </c>
-      <c r="N12" t="n">
-        <v>79</v>
-      </c>
-      <c r="O12" t="n">
-        <v>48</v>
-      </c>
-      <c r="P12" t="n">
-        <v>52</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>1.93</v>
-      </c>
-      <c r="R12" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="S12" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1.2</v>
-      </c>
       <c r="U12" t="n">
-        <v>1.76</v>
+        <v>1.88</v>
       </c>
       <c r="V12" t="n">
-        <v>2.68</v>
+        <v>3.15</v>
       </c>
       <c r="W12" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="AA12" t="n">
         <v>1.65</v>
       </c>
-      <c r="X12" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>1.6</v>
-      </c>
       <c r="AB12" t="n">
-        <v>1.93</v>
+        <v>1.95</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="AD12" t="n">
-        <v>2.44</v>
+        <v>2.7</v>
       </c>
       <c r="AE12" t="n">
-        <v>3.3</v>
+        <v>2.88</v>
       </c>
       <c r="AF12" t="n">
-        <v>1.51</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:30:00</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Inter Milan</t>
+          <t>Torque</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Kairat</t>
+          <t>Peñarol</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>1.36</v>
       </c>
       <c r="F13" t="n">
-        <v>1.18</v>
+        <v>2.05</v>
       </c>
       <c r="G13" t="n">
-        <v>1.96</v>
+        <v>1.55</v>
       </c>
       <c r="H13" t="n">
-        <v>1.37</v>
+        <v>1.78</v>
       </c>
       <c r="I13" t="n">
         <v>3.33</v>
       </c>
       <c r="J13" t="n">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="K13" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L13" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="M13" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N13" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O13" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P13" t="n">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.01</v>
+        <v>3.1</v>
       </c>
       <c r="R13" t="n">
-        <v>16</v>
+        <v>3.25</v>
       </c>
       <c r="S13" t="n">
-        <v>36</v>
+        <v>2.1</v>
       </c>
       <c r="T13" t="n">
-        <v>1.06</v>
+        <v>1.3</v>
       </c>
       <c r="U13" t="n">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>1.53</v>
+        <v>3.2</v>
       </c>
       <c r="W13" t="n">
-        <v>2.63</v>
+        <v>1.71</v>
       </c>
       <c r="X13" t="n">
-        <v>1.44</v>
+        <v>2</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.51</v>
+        <v>2.05</v>
       </c>
       <c r="Z13" t="n">
-        <v>2.01</v>
+        <v>1.76</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.45</v>
+        <v>1.57</v>
       </c>
       <c r="AB13" t="n">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="AC13" t="n">
-        <v>1.15</v>
+        <v>1.36</v>
       </c>
       <c r="AD13" t="n">
-        <v>1.62</v>
+        <v>2.78</v>
       </c>
       <c r="AE13" t="n">
-        <v>5</v>
+        <v>2.77</v>
       </c>
       <c r="AF13" t="n">
-        <v>2.08</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:45:00</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Olympique Marseille</t>
+          <t>Olympique Lyonnais</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>PSG</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="F14" t="n">
-        <v>1.33</v>
+        <v>1.83</v>
       </c>
       <c r="G14" t="n">
-        <v>1.22</v>
+        <v>1.51</v>
       </c>
       <c r="H14" t="n">
-        <v>1.62</v>
+        <v>1.98</v>
       </c>
       <c r="I14" t="n">
-        <v>2.84</v>
+        <v>3.49</v>
       </c>
       <c r="J14" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K14" t="n">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="L14" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="M14" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="N14" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="O14" t="n">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="P14" t="n">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="Q14" t="n">
-        <v>2.41</v>
+        <v>4.5</v>
       </c>
       <c r="R14" t="n">
-        <v>3.65</v>
+        <v>3.9</v>
       </c>
       <c r="S14" t="n">
-        <v>2.87</v>
+        <v>1.78</v>
       </c>
       <c r="T14" t="n">
-        <v>1.22</v>
+        <v>1.19</v>
       </c>
       <c r="U14" t="n">
-        <v>1.77</v>
+        <v>1.73</v>
       </c>
       <c r="V14" t="n">
-        <v>2.6</v>
+        <v>2.75</v>
       </c>
       <c r="W14" t="n">
-        <v>1.62</v>
+        <v>1.72</v>
       </c>
       <c r="X14" t="n">
-        <v>2.2</v>
+        <v>2.21</v>
       </c>
       <c r="Y14" t="n">
-        <v>2.05</v>
+        <v>2.37</v>
       </c>
       <c r="Z14" t="n">
-        <v>1.64</v>
+        <v>1.88</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.72</v>
+        <v>1.56</v>
       </c>
       <c r="AB14" t="n">
-        <v>2.5</v>
+        <v>1.92</v>
       </c>
       <c r="AC14" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="AD14" t="n">
-        <v>2.56</v>
+        <v>2.57</v>
       </c>
       <c r="AE14" t="n">
-        <v>3.5</v>
+        <v>3.35</v>
       </c>
       <c r="AF14" t="n">
-        <v>1.53</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-05 20:00:00</t>
+          <t>2025-11-09 19:45:00</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Newcastle United</t>
+          <t>Inter Milan</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Athletic Club Bilbao</t>
+          <t>Lazio</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
       </c>
       <c r="G15" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="J15" t="n">
+        <v>30</v>
+      </c>
+      <c r="K15" t="n">
+        <v>50</v>
+      </c>
+      <c r="L15" t="n">
+        <v>40</v>
+      </c>
+      <c r="M15" t="n">
+        <v>30</v>
+      </c>
+      <c r="N15" t="n">
+        <v>70</v>
+      </c>
+      <c r="O15" t="n">
+        <v>60</v>
+      </c>
+      <c r="P15" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="R15" t="n">
+        <v>5</v>
+      </c>
+      <c r="S15" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="U15" t="n">
         <v>1.74</v>
       </c>
-      <c r="H15" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="J15" t="n">
-        <v>50</v>
-      </c>
-      <c r="K15" t="n">
-        <v>67</v>
-      </c>
-      <c r="L15" t="n">
-        <v>33</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>100</v>
-      </c>
-      <c r="O15" t="n">
-        <v>84</v>
-      </c>
-      <c r="P15" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R15" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="S15" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="T15" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="U15" t="n">
-        <v>1.84</v>
-      </c>
       <c r="V15" t="n">
-        <v>2.95</v>
+        <v>2.7</v>
       </c>
       <c r="W15" t="n">
-        <v>1.95</v>
+        <v>2.02</v>
       </c>
       <c r="X15" t="n">
         <v>1.75</v>
       </c>
       <c r="Y15" t="n">
-        <v>2.62</v>
+        <v>2.35</v>
       </c>
       <c r="Z15" t="n">
-        <v>2.06</v>
+        <v>1.83</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.43</v>
+        <v>1.53</v>
       </c>
       <c r="AB15" t="n">
-        <v>1.74</v>
+        <v>1.87</v>
       </c>
       <c r="AC15" t="n">
-        <v>1.36</v>
+        <v>1.3</v>
       </c>
       <c r="AD15" t="n">
-        <v>2.5</v>
+        <v>2.44</v>
       </c>
       <c r="AE15" t="n">
-        <v>3.28</v>
+        <v>3.25</v>
       </c>
       <c r="AF15" t="n">
-        <v>1.49</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-05 22:00:00</t>
+          <t>2025-11-09 20:00:00</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Criciúma</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Atlético GO</t>
         </is>
       </c>
       <c r="E16" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="n">
+        <v>53</v>
+      </c>
+      <c r="K16" t="n">
+        <v>62</v>
+      </c>
+      <c r="L16" t="n">
+        <v>39</v>
+      </c>
+      <c r="M16" t="n">
+        <v>29</v>
+      </c>
+      <c r="N16" t="n">
+        <v>71</v>
+      </c>
+      <c r="O16" t="n">
+        <v>47</v>
+      </c>
+      <c r="P16" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="R16" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="S16" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="U16" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="V16" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="W16" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="X16" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="AC16" t="n">
         <v>1.47</v>
       </c>
-      <c r="F16" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="I16" t="n">
-        <v>2.53</v>
-      </c>
-      <c r="J16" t="n">
-        <v>52</v>
-      </c>
-      <c r="K16" t="n">
-        <v>71</v>
-      </c>
-      <c r="L16" t="n">
-        <v>32</v>
-      </c>
-      <c r="M16" t="n">
-        <v>32</v>
-      </c>
-      <c r="N16" t="n">
-        <v>68</v>
-      </c>
-      <c r="O16" t="n">
-        <v>46</v>
-      </c>
-      <c r="P16" t="n">
-        <v>55</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="R16" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="S16" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="T16" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="U16" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="V16" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1.85</v>
-      </c>
-      <c r="X16" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>1.48</v>
-      </c>
       <c r="AD16" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="AE16" t="n">
         <v>2.47</v>
       </c>
       <c r="AF16" t="n">
-        <v>1.29</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-05 22:00:00</t>
+          <t>2025-11-09 20:00:00</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vitória</t>
+          <t>Celta de Vigo</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>FC Barcelona</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>1.53</v>
+        <v>0.83</v>
       </c>
       <c r="F17" t="n">
-        <v>0.73</v>
+        <v>1.67</v>
       </c>
       <c r="G17" t="n">
-        <v>1.48</v>
+        <v>1.51</v>
       </c>
       <c r="H17" t="n">
-        <v>1.05</v>
+        <v>2.19</v>
       </c>
       <c r="I17" t="n">
-        <v>2.53</v>
+        <v>3.7</v>
       </c>
       <c r="J17" t="n">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="K17" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L17" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="M17" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="O17" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P17" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="Q17" t="n">
-        <v>2.31</v>
+        <v>3.75</v>
       </c>
       <c r="R17" t="n">
-        <v>2.9</v>
+        <v>4.18</v>
       </c>
       <c r="S17" t="n">
-        <v>2.87</v>
+        <v>1.7</v>
       </c>
       <c r="T17" t="n">
-        <v>1.36</v>
+        <v>1.06</v>
       </c>
       <c r="U17" t="n">
-        <v>2.31</v>
+        <v>1.4</v>
       </c>
       <c r="V17" t="n">
-        <v>4.35</v>
+        <v>2.04</v>
       </c>
       <c r="W17" t="n">
-        <v>1.89</v>
+        <v>1.4</v>
       </c>
       <c r="X17" t="n">
-        <v>1.83</v>
+        <v>3.05</v>
       </c>
       <c r="Y17" t="n">
-        <v>2.27</v>
+        <v>2.61</v>
       </c>
       <c r="Z17" t="n">
-        <v>1.81</v>
+        <v>1.98</v>
       </c>
       <c r="AA17" t="n">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="AB17" t="n">
-        <v>2.22</v>
+        <v>1.8</v>
       </c>
       <c r="AC17" t="n">
-        <v>1.47</v>
+        <v>1.2</v>
       </c>
       <c r="AD17" t="n">
-        <v>3.22</v>
+        <v>2.05</v>
       </c>
       <c r="AE17" t="n">
-        <v>2.5</v>
+        <v>4.33</v>
       </c>
       <c r="AF17" t="n">
-        <v>1.3</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-05 22:00:00</t>
+          <t>2025-11-09 20:00:00</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Real Valladolid</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.71</v>
+        <v>2.17</v>
       </c>
       <c r="F18" t="n">
-        <v>0.33</v>
+        <v>1.6</v>
       </c>
       <c r="G18" t="n">
-        <v>1.42</v>
+        <v>1.3</v>
       </c>
       <c r="H18" t="n">
-        <v>0.92</v>
+        <v>1.35</v>
       </c>
       <c r="I18" t="n">
-        <v>2.34</v>
+        <v>2.65</v>
       </c>
       <c r="J18" t="n">
+        <v>37</v>
+      </c>
+      <c r="K18" t="n">
         <v>45</v>
       </c>
-      <c r="K18" t="n">
-        <v>69</v>
-      </c>
       <c r="L18" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="M18" t="n">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="N18" t="n">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="O18" t="n">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="P18" t="n">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="Q18" t="n">
-        <v>1.7</v>
+        <v>2.9</v>
       </c>
       <c r="R18" t="n">
-        <v>3.4</v>
+        <v>2.95</v>
       </c>
       <c r="S18" t="n">
-        <v>4.15</v>
+        <v>2.5</v>
       </c>
       <c r="T18" t="n">
-        <v>1.24</v>
+        <v>1.39</v>
       </c>
       <c r="U18" t="n">
-        <v>1.93</v>
+        <v>2.38</v>
       </c>
       <c r="V18" t="n">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="W18" t="n">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="X18" t="n">
-        <v>1.88</v>
+        <v>1.77</v>
       </c>
       <c r="Y18" t="n">
-        <v>2.7</v>
+        <v>2.08</v>
       </c>
       <c r="Z18" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AB18" t="n">
         <v>2.11</v>
       </c>
-      <c r="AA18" t="n">
-        <v>1.41</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>1.66</v>
-      </c>
       <c r="AC18" t="n">
-        <v>1.36</v>
+        <v>1.5</v>
       </c>
       <c r="AD18" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="AE18" t="n">
-        <v>2.89</v>
+        <v>2.42</v>
       </c>
       <c r="AF18" t="n">
-        <v>1.41</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-05 22:30:00</t>
+          <t>2025-11-09 20:30:00</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Botafogo</t>
+          <t>Lusitania Lourosa</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Vasco da Gama</t>
+          <t>União de Leiria</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.73</v>
+        <v>0.8</v>
       </c>
       <c r="F19" t="n">
-        <v>1.13</v>
+        <v>1.6</v>
       </c>
       <c r="G19" t="n">
-        <v>1.68</v>
+        <v>1.72</v>
       </c>
       <c r="H19" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="I19" t="n">
-        <v>3.01</v>
+        <v>3.04</v>
       </c>
       <c r="J19" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="K19" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="L19" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M19" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="N19" t="n">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="O19" t="n">
+        <v>40</v>
+      </c>
+      <c r="P19" t="n">
         <v>60</v>
       </c>
-      <c r="P19" t="n">
-        <v>40</v>
-      </c>
       <c r="Q19" t="n">
-        <v>1.88</v>
+        <v>3</v>
       </c>
       <c r="R19" t="n">
-        <v>3.45</v>
+        <v>3.05</v>
       </c>
       <c r="S19" t="n">
-        <v>4</v>
+        <v>2.2</v>
       </c>
       <c r="T19" t="n">
-        <v>1.24</v>
+        <v>1.28</v>
       </c>
       <c r="U19" t="n">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="V19" t="n">
-        <v>3.08</v>
+        <v>3.68</v>
       </c>
       <c r="W19" t="n">
-        <v>1.75</v>
+        <v>1.89</v>
       </c>
       <c r="X19" t="n">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="Y19" t="n">
-        <v>2.34</v>
+        <v>2.74</v>
       </c>
       <c r="Z19" t="n">
-        <v>1.84</v>
+        <v>2.08</v>
       </c>
       <c r="AA19" t="n">
-        <v>1.56</v>
+        <v>1.36</v>
       </c>
       <c r="AB19" t="n">
-        <v>2.19</v>
+        <v>1.66</v>
       </c>
       <c r="AC19" t="n">
-        <v>1.38</v>
+        <v>1.42</v>
       </c>
       <c r="AD19" t="n">
-        <v>2.73</v>
+        <v>3.1</v>
       </c>
       <c r="AE19" t="n">
-        <v>2.81</v>
+        <v>2.5</v>
       </c>
       <c r="AF19" t="n">
-        <v>1.41</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-05 23:00:00</t>
+          <t>2025-11-09 20:30:00</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Atlético Mineiro</t>
+          <t>Benfica</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Casa Pia</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1.93</v>
+        <v>2.2</v>
       </c>
       <c r="F20" t="n">
-        <v>0.87</v>
+        <v>1.2</v>
       </c>
       <c r="G20" t="n">
-        <v>1.76</v>
+        <v>2.15</v>
       </c>
       <c r="H20" t="n">
-        <v>1.27</v>
+        <v>1.02</v>
       </c>
       <c r="I20" t="n">
-        <v>3.03</v>
+        <v>3.17</v>
       </c>
       <c r="J20" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="K20" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="L20" t="n">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="M20" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O20" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="P20" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="Q20" t="n">
-        <v>2.1</v>
+        <v>1.15</v>
       </c>
       <c r="R20" t="n">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="S20" t="n">
-        <v>3.4</v>
+        <v>13</v>
       </c>
       <c r="T20" t="n">
-        <v>1.38</v>
+        <v>1.17</v>
       </c>
       <c r="U20" t="n">
-        <v>2.19</v>
+        <v>1.62</v>
       </c>
       <c r="V20" t="n">
-        <v>3.8</v>
+        <v>2.6</v>
       </c>
       <c r="W20" t="n">
-        <v>1.96</v>
+        <v>2.38</v>
       </c>
       <c r="X20" t="n">
-        <v>1.85</v>
+        <v>1.53</v>
       </c>
       <c r="Y20" t="n">
-        <v>2.24</v>
+        <v>2.7</v>
       </c>
       <c r="Z20" t="n">
-        <v>1.77</v>
+        <v>2.05</v>
       </c>
       <c r="AA20" t="n">
-        <v>1.59</v>
+        <v>1.41</v>
       </c>
       <c r="AB20" t="n">
-        <v>1.95</v>
+        <v>1.68</v>
       </c>
       <c r="AC20" t="n">
-        <v>1.43</v>
+        <v>1.28</v>
       </c>
       <c r="AD20" t="n">
-        <v>2.88</v>
+        <v>2.4</v>
       </c>
       <c r="AE20" t="n">
-        <v>2.62</v>
+        <v>3.25</v>
       </c>
       <c r="AF20" t="n">
-        <v>1.33</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-05 23:00:00</t>
+          <t>2025-11-09 20:30:00</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Grêmio</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Moreirense FC</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1.73</v>
+        <v>1.4</v>
       </c>
       <c r="F21" t="n">
-        <v>1.47</v>
+        <v>1.2</v>
       </c>
       <c r="G21" t="n">
-        <v>1.38</v>
+        <v>1.61</v>
       </c>
       <c r="H21" t="n">
-        <v>1.26</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="I21" t="n">
-        <v>2.64</v>
+        <v>2.42</v>
       </c>
       <c r="J21" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K21" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="L21" t="n">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="M21" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N21" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O21" t="n">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="P21" t="n">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="Q21" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="R21" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="S21" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="V21" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="W21" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="X21" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AE21" t="n">
         <v>3</v>
       </c>
-      <c r="R21" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S21" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="T21" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="U21" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="V21" t="n">
-        <v>3.95</v>
-      </c>
-      <c r="W21" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="X21" t="n">
-        <v>1.85</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>2.58</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="AE21" t="n">
-        <v>2.59</v>
-      </c>
       <c r="AF21" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-06 00:30:00</t>
+          <t>2025-11-09 21:10:00</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Alianza Petrolera</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Flamengo</t>
+          <t>Boyacá Chicó</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1.8</v>
+        <v>1.45</v>
       </c>
       <c r="F22" t="n">
-        <v>1.86</v>
+        <v>0.95</v>
       </c>
       <c r="G22" t="n">
-        <v>1.39</v>
+        <v>1.36</v>
       </c>
       <c r="H22" t="n">
-        <v>1.45</v>
+        <v>1.14</v>
       </c>
       <c r="I22" t="n">
-        <v>2.84</v>
+        <v>2.5</v>
       </c>
       <c r="J22" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K22" t="n">
         <v>62</v>
       </c>
       <c r="L22" t="n">
+        <v>27</v>
+      </c>
+      <c r="M22" t="n">
+        <v>35</v>
+      </c>
+      <c r="N22" t="n">
+        <v>66</v>
+      </c>
+      <c r="O22" t="n">
+        <v>37</v>
+      </c>
+      <c r="P22" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="R22" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="S22" t="n">
+        <v>6</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="U22" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="V22" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="W22" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="X22" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-11-09 21:30:00</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>33</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Flamengo</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Santos</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="J23" t="n">
+        <v>41</v>
+      </c>
+      <c r="K23" t="n">
+        <v>60</v>
+      </c>
+      <c r="L23" t="n">
+        <v>25</v>
+      </c>
+      <c r="M23" t="n">
+        <v>28</v>
+      </c>
+      <c r="N23" t="n">
+        <v>72</v>
+      </c>
+      <c r="O23" t="n">
+        <v>50</v>
+      </c>
+      <c r="P23" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="R23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S23" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="V23" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="W23" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="X23" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-11-09 21:30:00</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>36</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CRB</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Operário PR</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="J24" t="n">
+        <v>38</v>
+      </c>
+      <c r="K24" t="n">
+        <v>68</v>
+      </c>
+      <c r="L24" t="n">
+        <v>36</v>
+      </c>
+      <c r="M24" t="n">
+        <v>35</v>
+      </c>
+      <c r="N24" t="n">
+        <v>65</v>
+      </c>
+      <c r="O24" t="n">
+        <v>35</v>
+      </c>
+      <c r="P24" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="R24" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="S24" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="U24" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="V24" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="W24" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="X24" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-11-09 22:20:00</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Banfield</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Aldosivi</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="J25" t="n">
+        <v>37</v>
+      </c>
+      <c r="K25" t="n">
+        <v>67</v>
+      </c>
+      <c r="L25" t="n">
+        <v>20</v>
+      </c>
+      <c r="M25" t="n">
+        <v>37</v>
+      </c>
+      <c r="N25" t="n">
+        <v>64</v>
+      </c>
+      <c r="O25" t="n">
+        <v>37</v>
+      </c>
+      <c r="P25" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="R25" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="S25" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="U25" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="V25" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="W25" t="n">
+        <v>2</v>
+      </c>
+      <c r="X25" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-11-09 22:20:00</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Sarmiento</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="J26" t="n">
+        <v>39</v>
+      </c>
+      <c r="K26" t="n">
+        <v>49</v>
+      </c>
+      <c r="L26" t="n">
+        <v>17</v>
+      </c>
+      <c r="M26" t="n">
+        <v>42</v>
+      </c>
+      <c r="N26" t="n">
+        <v>59</v>
+      </c>
+      <c r="O26" t="n">
+        <v>26</v>
+      </c>
+      <c r="P26" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="R26" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="S26" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="U26" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="V26" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="W26" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="X26" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-11-09 23:00:00</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>17</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Santos Laguna</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Pachuca</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="J27" t="n">
+        <v>47</v>
+      </c>
+      <c r="K27" t="n">
+        <v>75</v>
+      </c>
+      <c r="L27" t="n">
+        <v>41</v>
+      </c>
+      <c r="M27" t="n">
+        <v>28</v>
+      </c>
+      <c r="N27" t="n">
+        <v>72</v>
+      </c>
+      <c r="O27" t="n">
+        <v>57</v>
+      </c>
+      <c r="P27" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="R27" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="V27" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="W27" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="X27" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-11-09 23:20:00</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>19</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>América de Cali</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Unión Magdalena</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="J28" t="n">
+        <v>49</v>
+      </c>
+      <c r="K28" t="n">
+        <v>55</v>
+      </c>
+      <c r="L28" t="n">
+        <v>21</v>
+      </c>
+      <c r="M28" t="n">
+        <v>30</v>
+      </c>
+      <c r="N28" t="n">
+        <v>70</v>
+      </c>
+      <c r="O28" t="n">
+        <v>38</v>
+      </c>
+      <c r="P28" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="R28" t="n">
+        <v>5</v>
+      </c>
+      <c r="S28" t="n">
+        <v>9</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="U28" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="V28" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="W28" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="X28" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-11-09 23:30:00</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>33</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Mirassol</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Palmeiras</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>67</v>
+      </c>
+      <c r="K29" t="n">
+        <v>80</v>
+      </c>
+      <c r="L29" t="n">
+        <v>41</v>
+      </c>
+      <c r="M29" t="n">
+        <v>21</v>
+      </c>
+      <c r="N29" t="n">
+        <v>80</v>
+      </c>
+      <c r="O29" t="n">
+        <v>57</v>
+      </c>
+      <c r="P29" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="R29" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="U29" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="V29" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="W29" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="X29" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-11-09 23:30:00</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>33</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Grêmio</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="J30" t="n">
+        <v>41</v>
+      </c>
+      <c r="K30" t="n">
+        <v>82</v>
+      </c>
+      <c r="L30" t="n">
+        <v>35</v>
+      </c>
+      <c r="M30" t="n">
+        <v>25</v>
+      </c>
+      <c r="N30" t="n">
+        <v>75</v>
+      </c>
+      <c r="O30" t="n">
+        <v>35</v>
+      </c>
+      <c r="P30" t="n">
+        <v>66</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="R30" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="S30" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="U30" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="V30" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="X30" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-11-09 23:30:00</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>36</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Paysandu</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Coritiba</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="J31" t="n">
+        <v>44</v>
+      </c>
+      <c r="K31" t="n">
+        <v>59</v>
+      </c>
+      <c r="L31" t="n">
+        <v>27</v>
+      </c>
+      <c r="M31" t="n">
+        <v>50</v>
+      </c>
+      <c r="N31" t="n">
+        <v>50</v>
+      </c>
+      <c r="O31" t="n">
+        <v>33</v>
+      </c>
+      <c r="P31" t="n">
+        <v>68</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="R31" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="U31" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="V31" t="n">
+        <v>4</v>
+      </c>
+      <c r="W31" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="X31" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-11-10 00:30:00</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>15</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Atlético Tucumán</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="J32" t="n">
+        <v>37</v>
+      </c>
+      <c r="K32" t="n">
+        <v>77</v>
+      </c>
+      <c r="L32" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" t="n">
         <v>24</v>
       </c>
-      <c r="M22" t="n">
-        <v>28</v>
-      </c>
-      <c r="N22" t="n">
-        <v>72</v>
-      </c>
-      <c r="O22" t="n">
-        <v>38</v>
-      </c>
-      <c r="P22" t="n">
+      <c r="N32" t="n">
+        <v>77</v>
+      </c>
+      <c r="O32" t="n">
+        <v>47</v>
+      </c>
+      <c r="P32" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="R32" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="U32" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="V32" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="W32" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="X32" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-11-10 00:30:00</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>15</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tigre</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Estudiantes</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="J33" t="n">
+        <v>42</v>
+      </c>
+      <c r="K33" t="n">
+        <v>52</v>
+      </c>
+      <c r="L33" t="n">
+        <v>23</v>
+      </c>
+      <c r="M33" t="n">
+        <v>33</v>
+      </c>
+      <c r="N33" t="n">
+        <v>68</v>
+      </c>
+      <c r="O33" t="n">
+        <v>29</v>
+      </c>
+      <c r="P33" t="n">
+        <v>71</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="U33" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="V33" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="W33" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X33" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-11-10 01:30:00</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>19</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Santa Fe</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Deportivo Cali</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="J34" t="n">
+        <v>46</v>
+      </c>
+      <c r="K34" t="n">
+        <v>64</v>
+      </c>
+      <c r="L34" t="n">
+        <v>27</v>
+      </c>
+      <c r="M34" t="n">
+        <v>36</v>
+      </c>
+      <c r="N34" t="n">
+        <v>64</v>
+      </c>
+      <c r="O34" t="n">
+        <v>39</v>
+      </c>
+      <c r="P34" t="n">
         <v>62</v>
       </c>
-      <c r="Q22" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="R22" t="n">
-        <v>3.15</v>
-      </c>
-      <c r="S22" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="T22" t="n">
+      <c r="Q34" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="R34" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S34" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="U34" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="V34" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="W34" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="X34" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="AC34" t="n">
         <v>1.42</v>
       </c>
-      <c r="U22" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="V22" t="n">
-        <v>5.04</v>
-      </c>
-      <c r="W22" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="X22" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>2.32</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>1.94</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>2.39</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>1.32</v>
+      <c r="AD34" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-11-10 02:00:00</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Portland Timbers</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="J35" t="n">
+        <v>59</v>
+      </c>
+      <c r="K35" t="n">
+        <v>73</v>
+      </c>
+      <c r="L35" t="n">
+        <v>37</v>
+      </c>
+      <c r="M35" t="n">
+        <v>23</v>
+      </c>
+      <c r="N35" t="n">
+        <v>77</v>
+      </c>
+      <c r="O35" t="n">
+        <v>56</v>
+      </c>
+      <c r="P35" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="R35" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S35" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="U35" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="V35" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="W35" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="X35" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>